<commit_message>
added test cases for AAIR and VVIR
</commit_message>
<xml_diff>
--- a/simulink/TestCases_3k04.xlsx
+++ b/simulink/TestCases_3k04.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clara\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clara\Desktop\3K04_assignment2\SFWRENG-3K04\simulink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E349E71-5497-49C2-B28A-257CD47078BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39718F32-C410-4102-9E1E-F794CED9542C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{012ED018-E629-4E4C-B87E-D806D473D26F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{012ED018-E629-4E4C-B87E-D806D473D26F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>Actual Output</t>
   </si>
@@ -59,9 +59,6 @@
     <t>RATE = 70 bpm</t>
   </si>
   <si>
-    <t>ATR_amplitude = 3.5V</t>
-  </si>
-  <si>
     <t>NAT_HEART = 30 bpm</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>RATE = 60 pbm</t>
   </si>
   <si>
-    <t>VENT_amplitude = 3.8V</t>
-  </si>
-  <si>
     <t>ATR_PULSE_WIDTH = 10ms</t>
   </si>
   <si>
@@ -116,7 +110,79 @@
     <t>Recovery_time = 15sec</t>
   </si>
   <si>
-    <t>VRP = 250ms</t>
+    <t>ATR_Amplitude = 3.5V</t>
+  </si>
+  <si>
+    <t>NAT_HEART decreases to 60</t>
+  </si>
+  <si>
+    <t>VENT_Amplitude = 3.8V</t>
+  </si>
+  <si>
+    <t>High Threshold</t>
+  </si>
+  <si>
+    <t>Case 3</t>
+  </si>
+  <si>
+    <t>Mode = 7 (AAIR)</t>
+  </si>
+  <si>
+    <t>NAT_HEART increases to 100</t>
+  </si>
+  <si>
+    <t>RATE = 100</t>
+  </si>
+  <si>
+    <t>ATR_Amplitude = 3V</t>
+  </si>
+  <si>
+    <t>ATR_PULSE_WIDTH = 8ms</t>
+  </si>
+  <si>
+    <t>NAT_HEART = 90</t>
+  </si>
+  <si>
+    <t>Response_time = 10sec</t>
+  </si>
+  <si>
+    <t>Recovery_time = 10sec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATRSENSITIVITY_Amplitude = 1.5mV </t>
+  </si>
+  <si>
+    <t>Case 4</t>
+  </si>
+  <si>
+    <t>Mode 8 = VVIR</t>
+  </si>
+  <si>
+    <t>Boundry case, NAT_HEART remains constant at 65</t>
+  </si>
+  <si>
+    <t>RATE = 65</t>
+  </si>
+  <si>
+    <t>VENT_Amplitude = 5V</t>
+  </si>
+  <si>
+    <t>VENT_PULSE_WIDTH = 10ms</t>
+  </si>
+  <si>
+    <t>NAT_HEART = 65</t>
+  </si>
+  <si>
+    <t>Response_time = 5sec</t>
+  </si>
+  <si>
+    <t>Recovery_time = 5sec</t>
+  </si>
+  <si>
+    <t>VRP = 300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VENTSENSITIVITY_Amplitude = 2mV </t>
   </si>
 </sst>
 </file>
@@ -477,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AE6278-096E-4166-A87A-A018A589A3BD}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,7 +580,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -524,95 +590,212 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>14</v>
+      <c r="C13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>26</v>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added additional test cases, parameters changed
</commit_message>
<xml_diff>
--- a/simulink/TestCases_3k04.xlsx
+++ b/simulink/TestCases_3k04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clara\Desktop\3K04_assignment2\SFWRENG-3K04\simulink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39718F32-C410-4102-9E1E-F794CED9542C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4744FCEC-F442-422E-B52F-0A3C35AF0263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{012ED018-E629-4E4C-B87E-D806D473D26F}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{012ED018-E629-4E4C-B87E-D806D473D26F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="89">
   <si>
     <t>Actual Output</t>
   </si>
@@ -62,15 +62,9 @@
     <t>NAT_HEART = 30 bpm</t>
   </si>
   <si>
-    <t>Low Threshold</t>
-  </si>
-  <si>
     <t>Response_Factor = 8</t>
   </si>
   <si>
-    <t>ARP = 250ms</t>
-  </si>
-  <si>
     <t>NAT_HEART increases to 70 bpm slowly</t>
   </si>
   <si>
@@ -83,33 +77,15 @@
     <t>RATE = 60 pbm</t>
   </si>
   <si>
-    <t>ATR_PULSE_WIDTH = 10ms</t>
-  </si>
-  <si>
-    <t>VENT_PULSE_WIDTH = 5ms</t>
-  </si>
-  <si>
     <t>NAT_HEART = 140 bpm</t>
   </si>
   <si>
-    <t>Medium Threshold</t>
-  </si>
-  <si>
-    <t>Response_Factor = 5</t>
-  </si>
-  <si>
     <t>Reaction_time = 10sec</t>
   </si>
   <si>
     <t>Reaction_time = 30sec</t>
   </si>
   <si>
-    <t>Recovery_time = 300sec</t>
-  </si>
-  <si>
-    <t>Recovery_time = 15sec</t>
-  </si>
-  <si>
     <t>ATR_Amplitude = 3.5V</t>
   </si>
   <si>
@@ -119,36 +95,15 @@
     <t>VENT_Amplitude = 3.8V</t>
   </si>
   <si>
-    <t>High Threshold</t>
-  </si>
-  <si>
     <t>Case 3</t>
   </si>
   <si>
     <t>Mode = 7 (AAIR)</t>
   </si>
   <si>
-    <t>NAT_HEART increases to 100</t>
-  </si>
-  <si>
     <t>RATE = 100</t>
   </si>
   <si>
-    <t>ATR_Amplitude = 3V</t>
-  </si>
-  <si>
-    <t>ATR_PULSE_WIDTH = 8ms</t>
-  </si>
-  <si>
-    <t>NAT_HEART = 90</t>
-  </si>
-  <si>
-    <t>Response_time = 10sec</t>
-  </si>
-  <si>
-    <t>Recovery_time = 10sec</t>
-  </si>
-  <si>
     <t xml:space="preserve">ATRSENSITIVITY_Amplitude = 1.5mV </t>
   </si>
   <si>
@@ -167,22 +122,187 @@
     <t>VENT_Amplitude = 5V</t>
   </si>
   <si>
-    <t>VENT_PULSE_WIDTH = 10ms</t>
-  </si>
-  <si>
     <t>NAT_HEART = 65</t>
   </si>
   <si>
-    <t>Response_time = 5sec</t>
-  </si>
-  <si>
-    <t>Recovery_time = 5sec</t>
-  </si>
-  <si>
     <t>VRP = 300</t>
   </si>
   <si>
     <t xml:space="preserve">VENTSENSITIVITY_Amplitude = 2mV </t>
+  </si>
+  <si>
+    <t>Boundry case, NAT_HEART increases to 100</t>
+  </si>
+  <si>
+    <t>ATR_Amplitude = 4V</t>
+  </si>
+  <si>
+    <t>LRL = 60</t>
+  </si>
+  <si>
+    <t>URL = 120</t>
+  </si>
+  <si>
+    <t>Mode = 1 (AOO)</t>
+  </si>
+  <si>
+    <t>NAT_HEART Paces to LRL</t>
+  </si>
+  <si>
+    <t>VENT_Amplitude = 4V</t>
+  </si>
+  <si>
+    <t>Mode = 3 (AAI)</t>
+  </si>
+  <si>
+    <t>Case 5</t>
+  </si>
+  <si>
+    <t>Case 6</t>
+  </si>
+  <si>
+    <t>Case 7</t>
+  </si>
+  <si>
+    <t>Case 8</t>
+  </si>
+  <si>
+    <t>LRL = 40</t>
+  </si>
+  <si>
+    <t>URL = 60</t>
+  </si>
+  <si>
+    <t>VENT_PULSE_WIDTH = 0.1ms</t>
+  </si>
+  <si>
+    <t>VENT_Amplitude = 3.5V</t>
+  </si>
+  <si>
+    <t>ATR_PULSE_WIDTH = 0.12ms</t>
+  </si>
+  <si>
+    <t>NAT_HEART = 50 bpm</t>
+  </si>
+  <si>
+    <t>Mode = 2 (VOO)</t>
+  </si>
+  <si>
+    <t>ATR_Amplitude = 4.5V</t>
+  </si>
+  <si>
+    <t>ATR_PULSE_WIDTH = 1.5ms</t>
+  </si>
+  <si>
+    <t>ATRSENSITIVITY_Amplitude = 0.5mV</t>
+  </si>
+  <si>
+    <t>ARP = 150ms</t>
+  </si>
+  <si>
+    <t>NAT_HEART = 40 bpm</t>
+  </si>
+  <si>
+    <t>Mode = 4 (VVI)</t>
+  </si>
+  <si>
+    <t>VENT_PULSE_WIDTH = 1ms</t>
+  </si>
+  <si>
+    <t>VENTSENSITIVITY_Amplitude = 0.75mV</t>
+  </si>
+  <si>
+    <t>VRP = 400ms</t>
+  </si>
+  <si>
+    <t>LRL = 70</t>
+  </si>
+  <si>
+    <t>URL = 160</t>
+  </si>
+  <si>
+    <t>NAT_HEART = 80 bpm</t>
+  </si>
+  <si>
+    <t>NAT_HEART remains at 80, no pacing</t>
+  </si>
+  <si>
+    <t>ATR_PULSE_WIDTH = 0.3ms</t>
+  </si>
+  <si>
+    <t>Activity Threshold = Low</t>
+  </si>
+  <si>
+    <t>Activity Threshold = High</t>
+  </si>
+  <si>
+    <t>Activity Threshold = Medium</t>
+  </si>
+  <si>
+    <t>LRL = 50</t>
+  </si>
+  <si>
+    <t>URL = 110</t>
+  </si>
+  <si>
+    <t>MSR = 60 ppm</t>
+  </si>
+  <si>
+    <t>VENT_PULSE_WIDTH = 0.5ms</t>
+  </si>
+  <si>
+    <t>Response_Factor = 10</t>
+  </si>
+  <si>
+    <t>Recovery_time = 5min</t>
+  </si>
+  <si>
+    <t>ATR_Amplitude = 3.6V</t>
+  </si>
+  <si>
+    <t>ATR_PULSE_WIDTH = 1.8ms</t>
+  </si>
+  <si>
+    <t>NAT_HEART = 5</t>
+  </si>
+  <si>
+    <t>Response_Factor = 12</t>
+  </si>
+  <si>
+    <t>Recovery_time = 3min</t>
+  </si>
+  <si>
+    <t>MSR = 150</t>
+  </si>
+  <si>
+    <t>MSR = 120</t>
+  </si>
+  <si>
+    <t>URL = 100</t>
+  </si>
+  <si>
+    <t>Recovery_time = 12 min</t>
+  </si>
+  <si>
+    <t>Response_Factor = 15</t>
+  </si>
+  <si>
+    <t>Reaction_time = 38sec</t>
+  </si>
+  <si>
+    <t>VENT_PULSE_WIDTH = 1.7ms</t>
+  </si>
+  <si>
+    <t>MSR = 65</t>
+  </si>
+  <si>
+    <t>LRL = 75</t>
+  </si>
+  <si>
+    <t>URL = 165</t>
+  </si>
+  <si>
+    <t>Recovery_time = 8 min</t>
   </si>
 </sst>
 </file>
@@ -543,17 +663,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AE6278-096E-4166-A87A-A018A589A3BD}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" customWidth="1"/>
   </cols>
@@ -577,225 +697,448 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>31</v>
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>38</v>
+      <c r="B35" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B46" t="s">
-        <v>48</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" s="1"/>
+      <c r="B81" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test sequence model
</commit_message>
<xml_diff>
--- a/simulink/TestCases_3k04.xlsx
+++ b/simulink/TestCases_3k04.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pragy\Desktop\FALL 2022\SFWRENG 3K04\3K04_Assignment1\SFWRENG-3K04\simulink\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pragy\Desktop\FALL 2022\SFWRENG 3K04\3K04_Assignment1_new\SFWRENG-3K04\simulink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675C27D1-7D67-4AC9-BEAF-2614506A3FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC55873-22E4-4CB7-92E0-CB46FDFE231F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{012ED018-E629-4E4C-B87E-D806D473D26F}"/>
   </bookViews>
@@ -665,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AE6278-096E-4166-A87A-A018A589A3BD}">
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75:B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>